<commit_message>
added built JAR file
</commit_message>
<xml_diff>
--- a/TP-2/team builder results.xlsx
+++ b/TP-2/team builder results.xlsx
@@ -59,373 +59,373 @@
     <t>project00</t>
   </si>
   <si>
+    <t>EE08</t>
+  </si>
+  <si>
+    <t>ME03</t>
+  </si>
+  <si>
+    <t>ME05</t>
+  </si>
+  <si>
+    <t>ME25</t>
+  </si>
+  <si>
+    <t>project01</t>
+  </si>
+  <si>
+    <t>EE09</t>
+  </si>
+  <si>
+    <t>ME24</t>
+  </si>
+  <si>
+    <t>ME28</t>
+  </si>
+  <si>
+    <t>ME45</t>
+  </si>
+  <si>
+    <t>project02</t>
+  </si>
+  <si>
+    <t>EE02</t>
+  </si>
+  <si>
     <t>EE03</t>
   </si>
   <si>
-    <t>ME03</t>
+    <t>ME42</t>
+  </si>
+  <si>
+    <t>ME48</t>
+  </si>
+  <si>
+    <t>project03</t>
+  </si>
+  <si>
+    <t>EE07</t>
+  </si>
+  <si>
+    <t>ME35</t>
+  </si>
+  <si>
+    <t>ME53</t>
+  </si>
+  <si>
+    <t>ME57</t>
+  </si>
+  <si>
+    <t>project04</t>
+  </si>
+  <si>
+    <t>EE17</t>
+  </si>
+  <si>
+    <t>ME19</t>
+  </si>
+  <si>
+    <t>ME32</t>
+  </si>
+  <si>
+    <t>project05</t>
+  </si>
+  <si>
+    <t>EE00</t>
+  </si>
+  <si>
+    <t>ME39</t>
+  </si>
+  <si>
+    <t>ME50</t>
+  </si>
+  <si>
+    <t>ME60</t>
+  </si>
+  <si>
+    <t>project06</t>
+  </si>
+  <si>
+    <t>EE23</t>
   </si>
   <si>
     <t>ME09</t>
   </si>
   <si>
+    <t>ME23</t>
+  </si>
+  <si>
+    <t>ME40</t>
+  </si>
+  <si>
+    <t>project07</t>
+  </si>
+  <si>
+    <t>EE04</t>
+  </si>
+  <si>
+    <t>ME06</t>
+  </si>
+  <si>
+    <t>ME30</t>
+  </si>
+  <si>
+    <t>ME61</t>
+  </si>
+  <si>
+    <t>project08</t>
+  </si>
+  <si>
+    <t>EE06</t>
+  </si>
+  <si>
+    <t>ME37</t>
+  </si>
+  <si>
+    <t>ME52</t>
+  </si>
+  <si>
+    <t>ME63</t>
+  </si>
+  <si>
+    <t>project09</t>
+  </si>
+  <si>
+    <t>EE24</t>
+  </si>
+  <si>
+    <t>ME07</t>
+  </si>
+  <si>
+    <t>ME54</t>
+  </si>
+  <si>
+    <t>ME58</t>
+  </si>
+  <si>
+    <t>project10</t>
+  </si>
+  <si>
+    <t>EE10</t>
+  </si>
+  <si>
+    <t>ME04</t>
+  </si>
+  <si>
+    <t>ME10</t>
+  </si>
+  <si>
+    <t>ME62</t>
+  </si>
+  <si>
+    <t>project11</t>
+  </si>
+  <si>
+    <t>EE11</t>
+  </si>
+  <si>
+    <t>ME11</t>
+  </si>
+  <si>
+    <t>ME27</t>
+  </si>
+  <si>
+    <t>ME34</t>
+  </si>
+  <si>
+    <t>project12</t>
+  </si>
+  <si>
+    <t>EE12</t>
+  </si>
+  <si>
+    <t>ME12</t>
+  </si>
+  <si>
+    <t>ME33</t>
+  </si>
+  <si>
+    <t>ME44</t>
+  </si>
+  <si>
+    <t>project13</t>
+  </si>
+  <si>
+    <t>CpE01</t>
+  </si>
+  <si>
+    <t>CpE03</t>
+  </si>
+  <si>
+    <t>EE13</t>
+  </si>
+  <si>
+    <t>ME13</t>
+  </si>
+  <si>
+    <t>project14</t>
+  </si>
+  <si>
+    <t>EE14</t>
+  </si>
+  <si>
+    <t>ME14</t>
+  </si>
+  <si>
+    <t>ME46</t>
+  </si>
+  <si>
+    <t>ME47</t>
+  </si>
+  <si>
+    <t>project15</t>
+  </si>
+  <si>
+    <t>CpE00</t>
+  </si>
+  <si>
+    <t>EE15</t>
+  </si>
+  <si>
+    <t>ME15</t>
+  </si>
+  <si>
     <t>ME36</t>
   </si>
   <si>
-    <t>project01</t>
-  </si>
-  <si>
-    <t>EE24</t>
+    <t>project16</t>
+  </si>
+  <si>
+    <t>EE16</t>
+  </si>
+  <si>
+    <t>ME16</t>
+  </si>
+  <si>
+    <t>ME26</t>
+  </si>
+  <si>
+    <t>ME41</t>
+  </si>
+  <si>
+    <t>project17</t>
+  </si>
+  <si>
+    <t>EE01</t>
+  </si>
+  <si>
+    <t>ME00</t>
+  </si>
+  <si>
+    <t>ME17</t>
+  </si>
+  <si>
+    <t>ME49</t>
+  </si>
+  <si>
+    <t>ME55</t>
+  </si>
+  <si>
+    <t>project18</t>
+  </si>
+  <si>
+    <t>EE18</t>
   </si>
   <si>
     <t>ME02</t>
   </si>
   <si>
+    <t>ME18</t>
+  </si>
+  <si>
+    <t>ME59</t>
+  </si>
+  <si>
+    <t>project19</t>
+  </si>
+  <si>
+    <t>CpE02</t>
+  </si>
+  <si>
+    <t>EE19</t>
+  </si>
+  <si>
     <t>ME08</t>
   </si>
   <si>
-    <t>ME24</t>
-  </si>
-  <si>
-    <t>project02</t>
-  </si>
-  <si>
-    <t>EE02</t>
-  </si>
-  <si>
-    <t>EE06</t>
-  </si>
-  <si>
-    <t>ME05</t>
-  </si>
-  <si>
-    <t>ME34</t>
-  </si>
-  <si>
-    <t>project03</t>
-  </si>
-  <si>
-    <t>EE00</t>
+    <t>ME29</t>
+  </si>
+  <si>
+    <t>project20</t>
+  </si>
+  <si>
+    <t>EE20</t>
+  </si>
+  <si>
+    <t>ME21</t>
+  </si>
+  <si>
+    <t>ME31</t>
+  </si>
+  <si>
+    <t>ME56</t>
+  </si>
+  <si>
+    <t>project21</t>
+  </si>
+  <si>
+    <t>EE21</t>
+  </si>
+  <si>
+    <t>ME20</t>
+  </si>
+  <si>
+    <t>ME38</t>
   </si>
   <si>
     <t>ME43</t>
   </si>
   <si>
-    <t>ME44</t>
-  </si>
-  <si>
-    <t>ME58</t>
-  </si>
-  <si>
-    <t>project04</t>
-  </si>
-  <si>
-    <t>EE07</t>
+    <t>project22</t>
+  </si>
+  <si>
+    <t>EE05</t>
+  </si>
+  <si>
+    <t>EE22</t>
   </si>
   <si>
     <t>ME01</t>
   </si>
   <si>
-    <t>ME28</t>
-  </si>
-  <si>
-    <t>project05</t>
-  </si>
-  <si>
-    <t>EE05</t>
-  </si>
-  <si>
-    <t>ME42</t>
-  </si>
-  <si>
-    <t>ME55</t>
-  </si>
-  <si>
-    <t>ME62</t>
-  </si>
-  <si>
-    <t>project06</t>
-  </si>
-  <si>
-    <t>EE04</t>
-  </si>
-  <si>
-    <t>ME00</t>
-  </si>
-  <si>
-    <t>ME38</t>
-  </si>
-  <si>
-    <t>ME40</t>
-  </si>
-  <si>
-    <t>project07</t>
-  </si>
-  <si>
-    <t>EE08</t>
-  </si>
-  <si>
-    <t>ME27</t>
-  </si>
-  <si>
-    <t>ME29</t>
-  </si>
-  <si>
-    <t>ME31</t>
-  </si>
-  <si>
-    <t>project08</t>
-  </si>
-  <si>
-    <t>EE23</t>
-  </si>
-  <si>
-    <t>ME41</t>
-  </si>
-  <si>
-    <t>ME57</t>
-  </si>
-  <si>
-    <t>ME61</t>
-  </si>
-  <si>
-    <t>project09</t>
-  </si>
-  <si>
-    <t>EE01</t>
-  </si>
-  <si>
-    <t>ME07</t>
-  </si>
-  <si>
-    <t>ME39</t>
-  </si>
-  <si>
-    <t>ME50</t>
-  </si>
-  <si>
-    <t>project10</t>
-  </si>
-  <si>
-    <t>EE10</t>
-  </si>
-  <si>
-    <t>ME10</t>
-  </si>
-  <si>
-    <t>ME13</t>
-  </si>
-  <si>
-    <t>ME23</t>
-  </si>
-  <si>
-    <t>project11</t>
-  </si>
-  <si>
-    <t>EE11</t>
-  </si>
-  <si>
-    <t>ME06</t>
-  </si>
-  <si>
-    <t>ME11</t>
+    <t>ME22</t>
   </si>
   <si>
     <t>ME51</t>
   </si>
   <si>
-    <t>project12</t>
-  </si>
-  <si>
-    <t>EE12</t>
-  </si>
-  <si>
-    <t>ME12</t>
-  </si>
-  <si>
-    <t>ME20</t>
-  </si>
-  <si>
-    <t>ME46</t>
-  </si>
-  <si>
-    <t>project13</t>
-  </si>
-  <si>
-    <t>CpE02</t>
-  </si>
-  <si>
-    <t>CpE03</t>
-  </si>
-  <si>
-    <t>EE13</t>
-  </si>
-  <si>
-    <t>ME54</t>
-  </si>
-  <si>
-    <t>project14</t>
-  </si>
-  <si>
-    <t>EE14</t>
-  </si>
-  <si>
-    <t>ME14</t>
-  </si>
-  <si>
-    <t>ME26</t>
-  </si>
-  <si>
-    <t>ME35</t>
-  </si>
-  <si>
-    <t>project15</t>
-  </si>
-  <si>
-    <t>CpE00</t>
-  </si>
-  <si>
-    <t>EE15</t>
-  </si>
-  <si>
-    <t>ME04</t>
-  </si>
-  <si>
-    <t>ME15</t>
-  </si>
-  <si>
-    <t>project16</t>
-  </si>
-  <si>
-    <t>EE16</t>
-  </si>
-  <si>
-    <t>ME16</t>
-  </si>
-  <si>
-    <t>ME33</t>
-  </si>
-  <si>
-    <t>ME63</t>
-  </si>
-  <si>
-    <t>project17</t>
-  </si>
-  <si>
-    <t>EE17</t>
-  </si>
-  <si>
-    <t>ME17</t>
-  </si>
-  <si>
-    <t>ME48</t>
-  </si>
-  <si>
-    <t>ME59</t>
-  </si>
-  <si>
-    <t>ME60</t>
-  </si>
-  <si>
-    <t>project18</t>
-  </si>
-  <si>
-    <t>EE20</t>
-  </si>
-  <si>
-    <t>ME18</t>
-  </si>
-  <si>
-    <t>ME25</t>
-  </si>
-  <si>
-    <t>ME52</t>
-  </si>
-  <si>
-    <t>project19</t>
-  </si>
-  <si>
-    <t>CpE01</t>
-  </si>
-  <si>
-    <t>EE19</t>
-  </si>
-  <si>
-    <t>ME19</t>
-  </si>
-  <si>
-    <t>ME45</t>
-  </si>
-  <si>
-    <t>project20</t>
-  </si>
-  <si>
-    <t>EE18</t>
-  </si>
-  <si>
-    <t>ME30</t>
-  </si>
-  <si>
-    <t>ME32</t>
-  </si>
-  <si>
-    <t>ME56</t>
-  </si>
-  <si>
-    <t>project21</t>
-  </si>
-  <si>
-    <t>EE21</t>
-  </si>
-  <si>
-    <t>ME21</t>
-  </si>
-  <si>
-    <t>ME47</t>
-  </si>
-  <si>
-    <t>ME53</t>
-  </si>
-  <si>
-    <t>project22</t>
-  </si>
-  <si>
-    <t>EE09</t>
-  </si>
-  <si>
-    <t>EE22</t>
-  </si>
-  <si>
-    <t>ME22</t>
-  </si>
-  <si>
-    <t>ME37</t>
-  </si>
-  <si>
-    <t>ME49</t>
-  </si>
-  <si>
     <t>project23</t>
   </si>
   <si>
     <t>CE00</t>
   </si>
   <si>
+    <t>CE02</t>
+  </si>
+  <si>
+    <t>CE03</t>
+  </si>
+  <si>
+    <t>CE05</t>
+  </si>
+  <si>
+    <t>project24</t>
+  </si>
+  <si>
     <t>CE01</t>
   </si>
   <si>
-    <t>CE02</t>
-  </si>
-  <si>
     <t>CE04</t>
-  </si>
-  <si>
-    <t>project24</t>
-  </si>
-  <si>
-    <t>CE03</t>
-  </si>
-  <si>
-    <t>CE05</t>
   </si>
   <si>
     <t>CE06</t>
@@ -789,16 +789,16 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" t="n">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="I2" t="n">
         <v>3.3</v>
       </c>
       <c r="J2" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
       <c r="K2" t="n">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -826,16 +826,16 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" t="n">
-        <v>3.8</v>
+        <v>2.3</v>
       </c>
       <c r="I3" t="n">
-        <v>2.2</v>
+        <v>3.4</v>
       </c>
       <c r="J3" t="n">
         <v>3.8</v>
       </c>
       <c r="K3" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -866,13 +866,13 @@
         <v>3.6</v>
       </c>
       <c r="I4" t="n">
-        <v>3.0</v>
+        <v>3.7</v>
       </c>
       <c r="J4" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="K4" t="n">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -900,16 +900,16 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" t="n">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="I5" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J5" t="n">
         <v>3.3</v>
       </c>
-      <c r="J5" t="n">
-        <v>2.4</v>
-      </c>
       <c r="K5" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -938,10 +938,10 @@
         <v>3.1</v>
       </c>
       <c r="I6" t="n">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
       <c r="J6" t="n">
-        <v>3.8</v>
+        <v>2.2</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="9"/>
@@ -970,16 +970,16 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I7" t="n">
         <v>3.9</v>
       </c>
-      <c r="I7" t="n">
-        <v>2.2</v>
-      </c>
       <c r="J7" t="n">
-        <v>3.5</v>
+        <v>3.0</v>
       </c>
       <c r="K7" t="n">
-        <v>3.2</v>
+        <v>3.0</v>
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -1007,13 +1007,13 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="I8" t="n">
-        <v>2.0</v>
+        <v>2.9</v>
       </c>
       <c r="J8" t="n">
-        <v>3.8</v>
+        <v>3.3</v>
       </c>
       <c r="K8" t="n">
         <v>3.0</v>
@@ -1044,16 +1044,16 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" t="n">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="I9" t="n">
-        <v>2.7</v>
+        <v>3.6</v>
       </c>
       <c r="J9" t="n">
-        <v>3.9</v>
+        <v>3.0</v>
       </c>
       <c r="K9" t="n">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1081,16 +1081,16 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I10" t="n">
         <v>3.7</v>
       </c>
-      <c r="I10" t="n">
-        <v>3.1</v>
-      </c>
       <c r="J10" t="n">
-        <v>3.7</v>
+        <v>3.2</v>
       </c>
       <c r="K10" t="n">
-        <v>2.1</v>
+        <v>3.3</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
@@ -1118,16 +1118,16 @@
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" t="n">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="I11" t="n">
         <v>3.7</v>
       </c>
       <c r="J11" t="n">
-        <v>3.9</v>
+        <v>2.4</v>
       </c>
       <c r="K11" t="n">
-        <v>3.0</v>
+        <v>3.8</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
@@ -1158,13 +1158,13 @@
         <v>3.4</v>
       </c>
       <c r="I12" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="J12" t="n">
         <v>3.0</v>
       </c>
-      <c r="J12" t="n">
-        <v>3.3</v>
-      </c>
       <c r="K12" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -1195,13 +1195,13 @@
         <v>3.5</v>
       </c>
       <c r="I13" t="n">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="J13" t="n">
-        <v>3.1</v>
+        <v>2.7</v>
       </c>
       <c r="K13" t="n">
-        <v>3.1</v>
+        <v>3.4</v>
       </c>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
@@ -1235,10 +1235,10 @@
         <v>3.2</v>
       </c>
       <c r="J14" t="n">
-        <v>2.0</v>
+        <v>3.3</v>
       </c>
       <c r="K14" t="n">
-        <v>3.6</v>
+        <v>2.4</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -1266,7 +1266,7 @@
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" t="n">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="I15" t="n">
         <v>3.9</v>
@@ -1275,7 +1275,7 @@
         <v>2.7</v>
       </c>
       <c r="K15" t="n">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
@@ -1312,7 +1312,7 @@
         <v>3.6</v>
       </c>
       <c r="K16" t="n">
-        <v>2.5</v>
+        <v>3.7</v>
       </c>
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
@@ -1346,10 +1346,10 @@
         <v>3.9</v>
       </c>
       <c r="J17" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="K17" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="L17" s="31"/>
       <c r="M17" s="31"/>
@@ -1383,10 +1383,10 @@
         <v>3.6</v>
       </c>
       <c r="J18" t="n">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="K18" t="n">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -1416,19 +1416,19 @@
       </c>
       <c r="G19" s="35"/>
       <c r="H19" t="n">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="I19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J19" t="n">
         <v>3.7</v>
-      </c>
-      <c r="J19" t="n">
-        <v>2.8</v>
       </c>
       <c r="K19" t="n">
         <v>3.9</v>
       </c>
       <c r="L19" t="n">
-        <v>3.0</v>
+        <v>3.5</v>
       </c>
       <c r="M19" s="35"/>
       <c r="N19" t="n">
@@ -1455,16 +1455,16 @@
       <c r="F20" s="37"/>
       <c r="G20" s="37"/>
       <c r="H20" t="n">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="I20" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J20" t="n">
         <v>3.8</v>
       </c>
-      <c r="J20" t="n">
-        <v>3.5</v>
-      </c>
       <c r="K20" t="n">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="L20" s="37"/>
       <c r="M20" s="37"/>
@@ -1492,16 +1492,16 @@
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
       <c r="H21" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="I21" t="n">
         <v>2.3</v>
       </c>
       <c r="J21" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="K21" t="n">
         <v>3.9</v>
-      </c>
-      <c r="K21" t="n">
-        <v>3.5</v>
       </c>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
@@ -1529,13 +1529,13 @@
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="I22" t="n">
-        <v>3.0</v>
+        <v>3.1</v>
       </c>
       <c r="J22" t="n">
-        <v>2.2</v>
+        <v>3.1</v>
       </c>
       <c r="K22" t="n">
         <v>3.6</v>
@@ -1569,10 +1569,10 @@
         <v>3.5</v>
       </c>
       <c r="I23" t="n">
-        <v>3.1</v>
+        <v>2.0</v>
       </c>
       <c r="J23" t="n">
-        <v>3.7</v>
+        <v>3.8</v>
       </c>
       <c r="K23" t="n">
         <v>3.3</v>
@@ -1605,19 +1605,19 @@
       </c>
       <c r="G24" s="45"/>
       <c r="H24" t="n">
-        <v>2.3</v>
+        <v>3.9</v>
       </c>
       <c r="I24" t="n">
         <v>3.6</v>
       </c>
       <c r="J24" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="K24" t="n">
         <v>3.2</v>
       </c>
-      <c r="K24" t="n">
-        <v>3.7</v>
-      </c>
       <c r="L24" t="n">
-        <v>3.9</v>
+        <v>3.1</v>
       </c>
       <c r="M24" s="45"/>
       <c r="N24" t="n">
@@ -1647,13 +1647,13 @@
         <v>3.9</v>
       </c>
       <c r="I25" t="n">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="J25" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="K25" t="n">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="L25" s="47"/>
       <c r="M25" s="47"/>
@@ -1679,10 +1679,10 @@
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
       <c r="H26" t="n">
-        <v>3.2</v>
+        <v>2.7</v>
       </c>
       <c r="I26" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="J26" t="n">
         <v>3.5</v>

</xml_diff>

<commit_message>
added favorite projects to TeamBuilder, added content to HowToRun, changed some data in xls files
</commit_message>
<xml_diff>
--- a/TP-2/team builder results.xlsx
+++ b/TP-2/team builder results.xlsx
@@ -59,376 +59,376 @@
     <t>project00</t>
   </si>
   <si>
+    <t>EE00</t>
+  </si>
+  <si>
+    <t>ME25</t>
+  </si>
+  <si>
+    <t>ME30</t>
+  </si>
+  <si>
+    <t>ME62</t>
+  </si>
+  <si>
+    <t>project01</t>
+  </si>
+  <si>
+    <t>EE01</t>
+  </si>
+  <si>
+    <t>ME04</t>
+  </si>
+  <si>
+    <t>ME15</t>
+  </si>
+  <si>
+    <t>ME31</t>
+  </si>
+  <si>
+    <t>project02</t>
+  </si>
+  <si>
+    <t>EE02</t>
+  </si>
+  <si>
+    <t>EE23</t>
+  </si>
+  <si>
+    <t>ME32</t>
+  </si>
+  <si>
+    <t>ME59</t>
+  </si>
+  <si>
+    <t>project03</t>
+  </si>
+  <si>
+    <t>EE03</t>
+  </si>
+  <si>
+    <t>ME03</t>
+  </si>
+  <si>
+    <t>ME33</t>
+  </si>
+  <si>
+    <t>ME61</t>
+  </si>
+  <si>
+    <t>project04</t>
+  </si>
+  <si>
+    <t>EE04</t>
+  </si>
+  <si>
+    <t>ME34</t>
+  </si>
+  <si>
+    <t>ME54</t>
+  </si>
+  <si>
+    <t>project05</t>
+  </si>
+  <si>
+    <t>EE05</t>
+  </si>
+  <si>
+    <t>ME05</t>
+  </si>
+  <si>
+    <t>ME26</t>
+  </si>
+  <si>
+    <t>ME35</t>
+  </si>
+  <si>
+    <t>project06</t>
+  </si>
+  <si>
+    <t>EE06</t>
+  </si>
+  <si>
+    <t>ME06</t>
+  </si>
+  <si>
+    <t>ME36</t>
+  </si>
+  <si>
+    <t>ME56</t>
+  </si>
+  <si>
+    <t>project07</t>
+  </si>
+  <si>
+    <t>EE09</t>
+  </si>
+  <si>
+    <t>ME07</t>
+  </si>
+  <si>
+    <t>ME37</t>
+  </si>
+  <si>
+    <t>ME58</t>
+  </si>
+  <si>
+    <t>project08</t>
+  </si>
+  <si>
     <t>EE08</t>
   </si>
   <si>
-    <t>ME03</t>
-  </si>
-  <si>
-    <t>ME05</t>
-  </si>
-  <si>
-    <t>ME25</t>
-  </si>
-  <si>
-    <t>project01</t>
-  </si>
-  <si>
-    <t>EE09</t>
+    <t>ME02</t>
+  </si>
+  <si>
+    <t>ME08</t>
+  </si>
+  <si>
+    <t>ME38</t>
+  </si>
+  <si>
+    <t>project09</t>
+  </si>
+  <si>
+    <t>EE07</t>
+  </si>
+  <si>
+    <t>ME09</t>
+  </si>
+  <si>
+    <t>ME39</t>
+  </si>
+  <si>
+    <t>ME60</t>
+  </si>
+  <si>
+    <t>project10</t>
+  </si>
+  <si>
+    <t>EE10</t>
+  </si>
+  <si>
+    <t>ME10</t>
+  </si>
+  <si>
+    <t>ME40</t>
+  </si>
+  <si>
+    <t>ME53</t>
+  </si>
+  <si>
+    <t>project11</t>
+  </si>
+  <si>
+    <t>EE11</t>
+  </si>
+  <si>
+    <t>ME11</t>
+  </si>
+  <si>
+    <t>ME27</t>
+  </si>
+  <si>
+    <t>ME41</t>
+  </si>
+  <si>
+    <t>project12</t>
+  </si>
+  <si>
+    <t>EE12</t>
+  </si>
+  <si>
+    <t>ME12</t>
+  </si>
+  <si>
+    <t>ME42</t>
+  </si>
+  <si>
+    <t>ME63</t>
+  </si>
+  <si>
+    <t>project13</t>
+  </si>
+  <si>
+    <t>CpE00</t>
+  </si>
+  <si>
+    <t>CpE01</t>
+  </si>
+  <si>
+    <t>EE13</t>
+  </si>
+  <si>
+    <t>ME43</t>
+  </si>
+  <si>
+    <t>project14</t>
+  </si>
+  <si>
+    <t>EE14</t>
+  </si>
+  <si>
+    <t>ME14</t>
+  </si>
+  <si>
+    <t>ME44</t>
+  </si>
+  <si>
+    <t>ME57</t>
+  </si>
+  <si>
+    <t>project15</t>
+  </si>
+  <si>
+    <t>CpE02</t>
+  </si>
+  <si>
+    <t>EE15</t>
+  </si>
+  <si>
+    <t>ME01</t>
+  </si>
+  <si>
+    <t>ME45</t>
+  </si>
+  <si>
+    <t>project16</t>
+  </si>
+  <si>
+    <t>EE16</t>
+  </si>
+  <si>
+    <t>ME16</t>
   </si>
   <si>
     <t>ME24</t>
   </si>
   <si>
+    <t>ME46</t>
+  </si>
+  <si>
+    <t>project17</t>
+  </si>
+  <si>
+    <t>EE17</t>
+  </si>
+  <si>
+    <t>ME13</t>
+  </si>
+  <si>
+    <t>ME17</t>
+  </si>
+  <si>
+    <t>ME47</t>
+  </si>
+  <si>
+    <t>ME55</t>
+  </si>
+  <si>
+    <t>project18</t>
+  </si>
+  <si>
+    <t>EE18</t>
+  </si>
+  <si>
+    <t>ME00</t>
+  </si>
+  <si>
+    <t>ME18</t>
+  </si>
+  <si>
+    <t>ME48</t>
+  </si>
+  <si>
+    <t>project19</t>
+  </si>
+  <si>
+    <t>CpE03</t>
+  </si>
+  <si>
+    <t>EE19</t>
+  </si>
+  <si>
+    <t>ME19</t>
+  </si>
+  <si>
+    <t>ME49</t>
+  </si>
+  <si>
+    <t>project20</t>
+  </si>
+  <si>
+    <t>EE20</t>
+  </si>
+  <si>
+    <t>ME20</t>
+  </si>
+  <si>
+    <t>ME23</t>
+  </si>
+  <si>
+    <t>ME50</t>
+  </si>
+  <si>
+    <t>project21</t>
+  </si>
+  <si>
+    <t>EE21</t>
+  </si>
+  <si>
+    <t>ME21</t>
+  </si>
+  <si>
+    <t>ME29</t>
+  </si>
+  <si>
+    <t>ME51</t>
+  </si>
+  <si>
+    <t>project22</t>
+  </si>
+  <si>
+    <t>EE22</t>
+  </si>
+  <si>
+    <t>EE24</t>
+  </si>
+  <si>
+    <t>ME22</t>
+  </si>
+  <si>
     <t>ME28</t>
   </si>
   <si>
-    <t>ME45</t>
-  </si>
-  <si>
-    <t>project02</t>
-  </si>
-  <si>
-    <t>EE02</t>
-  </si>
-  <si>
-    <t>EE03</t>
-  </si>
-  <si>
-    <t>ME42</t>
-  </si>
-  <si>
-    <t>ME48</t>
-  </si>
-  <si>
-    <t>project03</t>
-  </si>
-  <si>
-    <t>EE07</t>
-  </si>
-  <si>
-    <t>ME35</t>
-  </si>
-  <si>
-    <t>ME53</t>
-  </si>
-  <si>
-    <t>ME57</t>
-  </si>
-  <si>
-    <t>project04</t>
-  </si>
-  <si>
-    <t>EE17</t>
-  </si>
-  <si>
-    <t>ME19</t>
-  </si>
-  <si>
-    <t>ME32</t>
-  </si>
-  <si>
-    <t>project05</t>
-  </si>
-  <si>
-    <t>EE00</t>
-  </si>
-  <si>
-    <t>ME39</t>
-  </si>
-  <si>
-    <t>ME50</t>
-  </si>
-  <si>
-    <t>ME60</t>
-  </si>
-  <si>
-    <t>project06</t>
-  </si>
-  <si>
-    <t>EE23</t>
-  </si>
-  <si>
-    <t>ME09</t>
-  </si>
-  <si>
-    <t>ME23</t>
-  </si>
-  <si>
-    <t>ME40</t>
-  </si>
-  <si>
-    <t>project07</t>
-  </si>
-  <si>
-    <t>EE04</t>
-  </si>
-  <si>
-    <t>ME06</t>
-  </si>
-  <si>
-    <t>ME30</t>
-  </si>
-  <si>
-    <t>ME61</t>
-  </si>
-  <si>
-    <t>project08</t>
-  </si>
-  <si>
-    <t>EE06</t>
-  </si>
-  <si>
-    <t>ME37</t>
-  </si>
-  <si>
     <t>ME52</t>
   </si>
   <si>
-    <t>ME63</t>
-  </si>
-  <si>
-    <t>project09</t>
-  </si>
-  <si>
-    <t>EE24</t>
-  </si>
-  <si>
-    <t>ME07</t>
-  </si>
-  <si>
-    <t>ME54</t>
-  </si>
-  <si>
-    <t>ME58</t>
-  </si>
-  <si>
-    <t>project10</t>
-  </si>
-  <si>
-    <t>EE10</t>
-  </si>
-  <si>
-    <t>ME04</t>
-  </si>
-  <si>
-    <t>ME10</t>
-  </si>
-  <si>
-    <t>ME62</t>
-  </si>
-  <si>
-    <t>project11</t>
-  </si>
-  <si>
-    <t>EE11</t>
-  </si>
-  <si>
-    <t>ME11</t>
-  </si>
-  <si>
-    <t>ME27</t>
-  </si>
-  <si>
-    <t>ME34</t>
-  </si>
-  <si>
-    <t>project12</t>
-  </si>
-  <si>
-    <t>EE12</t>
-  </si>
-  <si>
-    <t>ME12</t>
-  </si>
-  <si>
-    <t>ME33</t>
-  </si>
-  <si>
-    <t>ME44</t>
-  </si>
-  <si>
-    <t>project13</t>
-  </si>
-  <si>
-    <t>CpE01</t>
-  </si>
-  <si>
-    <t>CpE03</t>
-  </si>
-  <si>
-    <t>EE13</t>
-  </si>
-  <si>
-    <t>ME13</t>
-  </si>
-  <si>
-    <t>project14</t>
-  </si>
-  <si>
-    <t>EE14</t>
-  </si>
-  <si>
-    <t>ME14</t>
-  </si>
-  <si>
-    <t>ME46</t>
-  </si>
-  <si>
-    <t>ME47</t>
-  </si>
-  <si>
-    <t>project15</t>
-  </si>
-  <si>
-    <t>CpE00</t>
-  </si>
-  <si>
-    <t>EE15</t>
-  </si>
-  <si>
-    <t>ME15</t>
-  </si>
-  <si>
-    <t>ME36</t>
-  </si>
-  <si>
-    <t>project16</t>
-  </si>
-  <si>
-    <t>EE16</t>
-  </si>
-  <si>
-    <t>ME16</t>
-  </si>
-  <si>
-    <t>ME26</t>
-  </si>
-  <si>
-    <t>ME41</t>
-  </si>
-  <si>
-    <t>project17</t>
-  </si>
-  <si>
-    <t>EE01</t>
-  </si>
-  <si>
-    <t>ME00</t>
-  </si>
-  <si>
-    <t>ME17</t>
-  </si>
-  <si>
-    <t>ME49</t>
-  </si>
-  <si>
-    <t>ME55</t>
-  </si>
-  <si>
-    <t>project18</t>
-  </si>
-  <si>
-    <t>EE18</t>
-  </si>
-  <si>
-    <t>ME02</t>
-  </si>
-  <si>
-    <t>ME18</t>
-  </si>
-  <si>
-    <t>ME59</t>
-  </si>
-  <si>
-    <t>project19</t>
-  </si>
-  <si>
-    <t>CpE02</t>
-  </si>
-  <si>
-    <t>EE19</t>
-  </si>
-  <si>
-    <t>ME08</t>
-  </si>
-  <si>
-    <t>ME29</t>
-  </si>
-  <si>
-    <t>project20</t>
-  </si>
-  <si>
-    <t>EE20</t>
-  </si>
-  <si>
-    <t>ME21</t>
-  </si>
-  <si>
-    <t>ME31</t>
-  </si>
-  <si>
-    <t>ME56</t>
-  </si>
-  <si>
-    <t>project21</t>
-  </si>
-  <si>
-    <t>EE21</t>
-  </si>
-  <si>
-    <t>ME20</t>
-  </si>
-  <si>
-    <t>ME38</t>
-  </si>
-  <si>
-    <t>ME43</t>
-  </si>
-  <si>
-    <t>project22</t>
-  </si>
-  <si>
-    <t>EE05</t>
-  </si>
-  <si>
-    <t>EE22</t>
-  </si>
-  <si>
-    <t>ME01</t>
-  </si>
-  <si>
-    <t>ME22</t>
-  </si>
-  <si>
-    <t>ME51</t>
-  </si>
-  <si>
     <t>project23</t>
   </si>
   <si>
+    <t>CE03</t>
+  </si>
+  <si>
+    <t>CE04</t>
+  </si>
+  <si>
+    <t>CE05</t>
+  </si>
+  <si>
+    <t>CE06</t>
+  </si>
+  <si>
+    <t>project24</t>
+  </si>
+  <si>
     <t>CE00</t>
   </si>
   <si>
+    <t>CE01</t>
+  </si>
+  <si>
     <t>CE02</t>
-  </si>
-  <si>
-    <t>CE03</t>
-  </si>
-  <si>
-    <t>CE05</t>
-  </si>
-  <si>
-    <t>project24</t>
-  </si>
-  <si>
-    <t>CE01</t>
-  </si>
-  <si>
-    <t>CE04</t>
-  </si>
-  <si>
-    <t>CE06</t>
   </si>
 </sst>
 </file>
@@ -789,16 +789,16 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="K2" t="n">
         <v>3.2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K2" t="n">
-        <v>3.5</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -826,16 +826,16 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" t="n">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="I3" t="n">
         <v>3.4</v>
       </c>
       <c r="J3" t="n">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="K3" t="n">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -872,7 +872,7 @@
         <v>2.2</v>
       </c>
       <c r="K4" t="n">
-        <v>2.8</v>
+        <v>3.9</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
@@ -900,16 +900,16 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" t="n">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="I5" t="n">
-        <v>2.5</v>
+        <v>3.3</v>
       </c>
       <c r="J5" t="n">
         <v>3.3</v>
       </c>
       <c r="K5" t="n">
-        <v>3.7</v>
+        <v>2.1</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -935,13 +935,13 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" t="n">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
       <c r="I6" t="n">
-        <v>3.9</v>
+        <v>3.4</v>
       </c>
       <c r="J6" t="n">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="9"/>
@@ -970,16 +970,16 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" t="n">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="I7" t="n">
-        <v>3.9</v>
+        <v>2.5</v>
       </c>
       <c r="J7" t="n">
-        <v>3.0</v>
+        <v>3.6</v>
       </c>
       <c r="K7" t="n">
-        <v>3.0</v>
+        <v>2.5</v>
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
@@ -1007,16 +1007,16 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" t="n">
-        <v>3.7</v>
+        <v>3.0</v>
       </c>
       <c r="I8" t="n">
-        <v>2.9</v>
+        <v>3.6</v>
       </c>
       <c r="J8" t="n">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="K8" t="n">
-        <v>3.0</v>
+        <v>3.6</v>
       </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -1044,16 +1044,16 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K9" t="n">
         <v>3.8</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="J9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>2.1</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1081,16 +1081,16 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" t="n">
-        <v>3.0</v>
+        <v>3.2</v>
       </c>
       <c r="I10" t="n">
-        <v>3.7</v>
+        <v>2.2</v>
       </c>
       <c r="J10" t="n">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="K10" t="n">
-        <v>3.3</v>
+        <v>3.8</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
@@ -1118,16 +1118,16 @@
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" t="n">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
       <c r="I11" t="n">
-        <v>3.7</v>
+        <v>2.9</v>
       </c>
       <c r="J11" t="n">
-        <v>2.4</v>
+        <v>3.9</v>
       </c>
       <c r="K11" t="n">
-        <v>3.8</v>
+        <v>3.0</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
@@ -1158,13 +1158,13 @@
         <v>3.4</v>
       </c>
       <c r="I12" t="n">
-        <v>3.4</v>
+        <v>3.0</v>
       </c>
       <c r="J12" t="n">
         <v>3.0</v>
       </c>
       <c r="K12" t="n">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
@@ -1201,7 +1201,7 @@
         <v>2.7</v>
       </c>
       <c r="K13" t="n">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
@@ -1235,10 +1235,10 @@
         <v>3.2</v>
       </c>
       <c r="J14" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K14" t="n">
         <v>3.3</v>
-      </c>
-      <c r="K14" t="n">
-        <v>2.4</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -1266,10 +1266,10 @@
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="I15" t="n">
         <v>3.7</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3.9</v>
       </c>
       <c r="J15" t="n">
         <v>2.7</v>
@@ -1309,7 +1309,7 @@
         <v>2.4</v>
       </c>
       <c r="J16" t="n">
-        <v>3.6</v>
+        <v>2.4</v>
       </c>
       <c r="K16" t="n">
         <v>3.7</v>
@@ -1340,16 +1340,16 @@
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
       <c r="H17" t="n">
-        <v>2.6</v>
+        <v>3.8</v>
       </c>
       <c r="I17" t="n">
         <v>3.9</v>
       </c>
       <c r="J17" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="K17" t="n">
         <v>3.5</v>
-      </c>
-      <c r="K17" t="n">
-        <v>3.6</v>
       </c>
       <c r="L17" s="31"/>
       <c r="M17" s="31"/>
@@ -1383,10 +1383,10 @@
         <v>3.6</v>
       </c>
       <c r="J18" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="K18" t="n">
         <v>3.6</v>
-      </c>
-      <c r="K18" t="n">
-        <v>3.1</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -1416,16 +1416,16 @@
       </c>
       <c r="G19" s="35"/>
       <c r="H19" t="n">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="I19" t="n">
-        <v>2.0</v>
+        <v>3.3</v>
       </c>
       <c r="J19" t="n">
         <v>3.7</v>
       </c>
       <c r="K19" t="n">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="L19" t="n">
         <v>3.5</v>
@@ -1458,13 +1458,13 @@
         <v>3.2</v>
       </c>
       <c r="I20" t="n">
-        <v>2.2</v>
+        <v>3.0</v>
       </c>
       <c r="J20" t="n">
         <v>3.8</v>
       </c>
       <c r="K20" t="n">
-        <v>3.9</v>
+        <v>2.8</v>
       </c>
       <c r="L20" s="37"/>
       <c r="M20" s="37"/>
@@ -1492,13 +1492,13 @@
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
       <c r="H21" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="I21" t="n">
         <v>2.3</v>
       </c>
       <c r="J21" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="K21" t="n">
         <v>3.9</v>
@@ -1532,13 +1532,13 @@
         <v>3.4</v>
       </c>
       <c r="I22" t="n">
-        <v>3.1</v>
+        <v>3.0</v>
       </c>
       <c r="J22" t="n">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="K22" t="n">
-        <v>3.6</v>
+        <v>3.0</v>
       </c>
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
@@ -1569,13 +1569,13 @@
         <v>3.5</v>
       </c>
       <c r="I23" t="n">
-        <v>2.0</v>
+        <v>2.1</v>
       </c>
       <c r="J23" t="n">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="K23" t="n">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="L23" s="43"/>
       <c r="M23" s="43"/>
@@ -1605,19 +1605,19 @@
       </c>
       <c r="G24" s="45"/>
       <c r="H24" t="n">
-        <v>3.9</v>
+        <v>3.6</v>
       </c>
       <c r="I24" t="n">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="J24" t="n">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="K24" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="L24" t="n">
         <v>3.2</v>
-      </c>
-      <c r="L24" t="n">
-        <v>3.1</v>
       </c>
       <c r="M24" s="45"/>
       <c r="N24" t="n">
@@ -1644,16 +1644,16 @@
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
       <c r="H25" t="n">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
       <c r="I25" t="n">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="J25" t="n">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="K25" t="n">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="L25" s="47"/>
       <c r="M25" s="47"/>
@@ -1679,13 +1679,13 @@
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
       <c r="H26" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="I26" t="n">
         <v>2.7</v>
       </c>
-      <c r="I26" t="n">
-        <v>3.3</v>
-      </c>
       <c r="J26" t="n">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="K26" s="49"/>
       <c r="L26" s="49"/>

</xml_diff>